<commit_message>
update 2025-12-01 14:22:39 by win-g08qkcqo325
</commit_message>
<xml_diff>
--- a/utils/recordingExcel/GSR/GSR_Rat2RHD_LocalGlobal_RecordingAC.xlsx
+++ b/utils/recordingExcel/GSR/GSR_Rat2RHD_LocalGlobal_RecordingAC.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
-  <workbookPr filterPrivacy="true"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95CA359-74CA-4B64-87C3-09555551B8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A6F772-8490-494D-A284-4E5B20C3607E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="3120" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="5085" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="第一针" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="true"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="67147" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="433">
   <si>
     <t>RNP_Noise</t>
   </si>
@@ -1362,13 +1362,7 @@
   </si>
   <si>
     <t>A8o3M1o0_IC</t>
-  </si>
-  <si>
-    <t>A8o3M1o0_IC</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A8o3M1o3_IC</t>
   </si>
   <si>
     <t>A8o3M1o3_IC</t>
@@ -1376,13 +1370,7 @@
   </si>
   <si>
     <t>A8o3M1o6_IC</t>
-  </si>
-  <si>
-    <t>A8o3M1o6_IC</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A8o6M1o6_IC</t>
   </si>
   <si>
     <t>A8o6M1o6_IC</t>
@@ -1390,9 +1378,6 @@
   </si>
   <si>
     <t>A8o6M1o3_IC</t>
-  </si>
-  <si>
-    <t>A8o6M1o3_IC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1401,13 +1386,7 @@
   </si>
   <si>
     <t>A8o0M1o0_IC</t>
-  </si>
-  <si>
-    <t>A8o0M1o0_IC</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A8o0M1o3_IC</t>
   </si>
   <si>
     <t>A8o0M1o3_IC</t>
@@ -1421,11 +1400,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1465,7 +1444,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1595,67 +1574,65 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="true" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="1" quotePrefix="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="2" quotePrefix="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="2" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="2" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="1" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="样式 1" xfId="2"/>
-    <cellStyle name="样式 2" xfId="1"/>
+    <cellStyle name="样式 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="样式 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1671,7 +1648,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1788,7 +1765,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1812,9 +1789,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1838,7 +1815,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1873,7 +1850,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1891,7 +1868,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1916,7 +1893,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1932,37 +1909,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R170"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51:J56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.125" style="3" customWidth="true"/>
-    <col min="2" max="2" width="64" customWidth="true"/>
-    <col min="3" max="3" width="19.625" customWidth="true"/>
-    <col min="4" max="4" width="64.875" customWidth="true"/>
-    <col min="5" max="5" width="6.875" style="3" customWidth="true"/>
-    <col min="6" max="6" width="14.875" customWidth="true"/>
-    <col min="7" max="7" width="6.875" style="3" customWidth="true"/>
-    <col min="9" max="9" width="10.625" style="3" bestFit="true" customWidth="true"/>
-    <col min="10" max="10" width="11.375" style="3" customWidth="true"/>
-    <col min="11" max="11" width="7.5" customWidth="true"/>
-    <col min="12" max="12" width="7" customWidth="true"/>
-    <col min="13" max="13" width="10.875" style="4" customWidth="true"/>
-    <col min="14" max="14" width="5.625" style="3" customWidth="true"/>
-    <col min="15" max="15" width="6.875" customWidth="true"/>
-    <col min="16" max="16" width="8" style="3" customWidth="true"/>
-    <col min="17" max="17" width="5.625" style="3" customWidth="true"/>
-    <col min="18" max="18" width="9.75" customWidth="true"/>
-    <col min="19" max="19" width="34.875" customWidth="true"/>
-    <col min="8" max="8" width="6.875" style="3" customWidth="true"/>
+    <col min="1" max="1" width="3.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="64" customWidth="1"/>
+    <col min="3" max="3" width="19.625" customWidth="1"/>
+    <col min="4" max="4" width="64.875" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.875" customWidth="1"/>
+    <col min="7" max="8" width="6.875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="7.5" customWidth="1"/>
+    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="13" max="13" width="10.875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="5.625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="6.875" customWidth="1"/>
+    <col min="16" max="16" width="8" style="3" customWidth="1"/>
+    <col min="17" max="17" width="5.625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="9.75" customWidth="1"/>
+    <col min="19" max="19" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2018,7 +1994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -2074,7 +2050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" s="30" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
         <v>1</v>
       </c>
@@ -2091,7 +2067,7 @@
         <v>174</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>317</v>
@@ -2111,14 +2087,8 @@
       <c r="L3" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" s="30" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
         <v>1</v>
       </c>
@@ -2135,7 +2105,7 @@
         <v>174</v>
       </c>
       <c r="F4" s="46" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>317</v>
@@ -2155,14 +2125,8 @@
       <c r="L4" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -2179,7 +2143,7 @@
         <v>174</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>317</v>
@@ -2199,14 +2163,8 @@
       <c r="L5" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" s="30" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
         <v>1</v>
       </c>
@@ -2223,7 +2181,7 @@
         <v>174</v>
       </c>
       <c r="F6" s="46" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>317</v>
@@ -2243,14 +2201,8 @@
       <c r="L6" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" s="30" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="30">
         <v>1</v>
       </c>
@@ -2267,7 +2219,7 @@
         <v>174</v>
       </c>
       <c r="F7" s="46" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>317</v>
@@ -2287,14 +2239,8 @@
       <c r="L7" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" s="31" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="31">
         <v>1</v>
       </c>
@@ -2311,7 +2257,7 @@
         <v>174</v>
       </c>
       <c r="F8" s="46" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>317</v>
@@ -2331,14 +2277,8 @@
       <c r="L8" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -2355,7 +2295,7 @@
         <v>174</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>318</v>
@@ -2375,14 +2315,8 @@
       <c r="L9" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -2399,7 +2333,7 @@
         <v>174</v>
       </c>
       <c r="F10" s="46" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>318</v>
@@ -2419,14 +2353,8 @@
       <c r="L10" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>2</v>
       </c>
@@ -2443,7 +2371,7 @@
         <v>174</v>
       </c>
       <c r="F11" s="46" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>318</v>
@@ -2463,14 +2391,8 @@
       <c r="L11" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>2</v>
       </c>
@@ -2487,7 +2409,7 @@
         <v>174</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>318</v>
@@ -2507,14 +2429,8 @@
       <c r="L12" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" s="30" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="42">
         <v>2</v>
       </c>
@@ -2531,7 +2447,7 @@
         <v>174</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>318</v>
@@ -2551,14 +2467,8 @@
       <c r="L13" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" s="34" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="34">
         <v>2</v>
       </c>
@@ -2575,7 +2485,7 @@
         <v>174</v>
       </c>
       <c r="F14" s="46" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>318</v>
@@ -2595,14 +2505,8 @@
       <c r="L14" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="34"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="42">
         <v>3</v>
       </c>
@@ -2619,7 +2523,7 @@
         <v>174</v>
       </c>
       <c r="F15" s="46" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>319</v>
@@ -2639,14 +2543,8 @@
       <c r="L15" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>3</v>
       </c>
@@ -2663,7 +2561,7 @@
         <v>174</v>
       </c>
       <c r="F16" s="46" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>319</v>
@@ -2683,14 +2581,8 @@
       <c r="L16" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="42">
         <v>3</v>
       </c>
@@ -2707,7 +2599,7 @@
         <v>174</v>
       </c>
       <c r="F17" s="46" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>319</v>
@@ -2727,14 +2619,8 @@
       <c r="L17" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="42">
         <v>3</v>
       </c>
@@ -2751,7 +2637,7 @@
         <v>174</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>319</v>
@@ -2771,14 +2657,8 @@
       <c r="L18" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="42">
         <v>3</v>
       </c>
@@ -2795,7 +2675,7 @@
         <v>174</v>
       </c>
       <c r="F19" s="46" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>319</v>
@@ -2815,14 +2695,8 @@
       <c r="L19" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" s="34" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="34">
         <v>3</v>
       </c>
@@ -2839,7 +2713,7 @@
         <v>174</v>
       </c>
       <c r="F20" s="46" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>319</v>
@@ -2859,14 +2733,8 @@
       <c r="L20" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="43">
         <v>4</v>
       </c>
@@ -2883,7 +2751,7 @@
         <v>174</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>410</v>
@@ -2903,14 +2771,8 @@
       <c r="L21" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="43">
         <v>4</v>
       </c>
@@ -2927,7 +2789,7 @@
         <v>174</v>
       </c>
       <c r="F22" s="46" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>410</v>
@@ -2947,14 +2809,8 @@
       <c r="L22" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="43">
         <v>4</v>
       </c>
@@ -2971,7 +2827,7 @@
         <v>174</v>
       </c>
       <c r="F23" s="46" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>410</v>
@@ -2991,14 +2847,8 @@
       <c r="L23" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="43">
         <v>4</v>
       </c>
@@ -3015,7 +2865,7 @@
         <v>174</v>
       </c>
       <c r="F24" s="46" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>410</v>
@@ -3035,14 +2885,8 @@
       <c r="L24" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="43">
         <v>4</v>
       </c>
@@ -3059,7 +2903,7 @@
         <v>174</v>
       </c>
       <c r="F25" s="46" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>410</v>
@@ -3079,14 +2923,8 @@
       <c r="L25" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" s="34" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="34">
         <v>4</v>
       </c>
@@ -3103,7 +2941,7 @@
         <v>174</v>
       </c>
       <c r="F26" s="46" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>410</v>
@@ -3123,14 +2961,8 @@
       <c r="L26" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="43">
         <v>5</v>
       </c>
@@ -3147,7 +2979,7 @@
         <v>174</v>
       </c>
       <c r="F27" s="46" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>411</v>
@@ -3167,14 +2999,8 @@
       <c r="L27" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="43">
         <v>5</v>
       </c>
@@ -3191,7 +3017,7 @@
         <v>174</v>
       </c>
       <c r="F28" s="46" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>411</v>
@@ -3211,14 +3037,8 @@
       <c r="L28" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="29" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="43">
         <v>5</v>
       </c>
@@ -3235,7 +3055,7 @@
         <v>174</v>
       </c>
       <c r="F29" s="46" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>411</v>
@@ -3255,14 +3075,8 @@
       <c r="L29" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="43">
         <v>5</v>
       </c>
@@ -3279,7 +3093,7 @@
         <v>174</v>
       </c>
       <c r="F30" s="46" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>411</v>
@@ -3299,14 +3113,8 @@
       <c r="L30" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="31" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="43">
         <v>5</v>
       </c>
@@ -3323,7 +3131,7 @@
         <v>174</v>
       </c>
       <c r="F31" s="46" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>411</v>
@@ -3343,14 +3151,8 @@
       <c r="L31" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="32" s="34" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34">
         <v>5</v>
       </c>
@@ -3367,7 +3169,7 @@
         <v>174</v>
       </c>
       <c r="F32" s="46" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>411</v>
@@ -3387,14 +3189,8 @@
       <c r="L32" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="33" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="43">
         <v>6</v>
       </c>
@@ -3411,7 +3207,7 @@
         <v>174</v>
       </c>
       <c r="F33" s="46" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>412</v>
@@ -3431,14 +3227,8 @@
       <c r="L33" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="34" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="43">
         <v>6</v>
       </c>
@@ -3455,7 +3245,7 @@
         <v>174</v>
       </c>
       <c r="F34" s="46" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>412</v>
@@ -3475,14 +3265,8 @@
       <c r="L34" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="35" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="43">
         <v>6</v>
       </c>
@@ -3499,7 +3283,7 @@
         <v>174</v>
       </c>
       <c r="F35" s="46" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>412</v>
@@ -3519,14 +3303,8 @@
       <c r="L35" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="36" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="43">
         <v>6</v>
       </c>
@@ -3543,7 +3321,7 @@
         <v>174</v>
       </c>
       <c r="F36" s="46" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>412</v>
@@ -3563,14 +3341,8 @@
       <c r="L36" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="37" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="43">
         <v>6</v>
       </c>
@@ -3587,7 +3359,7 @@
         <v>174</v>
       </c>
       <c r="F37" s="46" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>412</v>
@@ -3607,14 +3379,8 @@
       <c r="L37" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="38" s="34" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="34">
         <v>6</v>
       </c>
@@ -3631,7 +3397,7 @@
         <v>174</v>
       </c>
       <c r="F38" s="46" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>412</v>
@@ -3651,14 +3417,8 @@
       <c r="L38" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
-      <c r="O38" s="34"/>
-      <c r="P38" s="34"/>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="34"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="39" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="43">
         <v>7</v>
       </c>
@@ -3675,7 +3435,7 @@
         <v>174</v>
       </c>
       <c r="F39" s="46" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>413</v>
@@ -3695,14 +3455,8 @@
       <c r="L39" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="40" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="43">
         <v>7</v>
       </c>
@@ -3719,7 +3473,7 @@
         <v>174</v>
       </c>
       <c r="F40" s="46" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>413</v>
@@ -3739,14 +3493,8 @@
       <c r="L40" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="41" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="43">
         <v>7</v>
       </c>
@@ -3763,7 +3511,7 @@
         <v>174</v>
       </c>
       <c r="F41" s="46" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>413</v>
@@ -3783,14 +3531,8 @@
       <c r="L41" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="42" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="43">
         <v>7</v>
       </c>
@@ -3807,7 +3549,7 @@
         <v>174</v>
       </c>
       <c r="F42" s="46" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>413</v>
@@ -3827,14 +3569,8 @@
       <c r="L42" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="43" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="43">
         <v>7</v>
       </c>
@@ -3851,7 +3587,7 @@
         <v>174</v>
       </c>
       <c r="F43" s="46" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>413</v>
@@ -3871,14 +3607,8 @@
       <c r="L43" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="44" s="31" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="43">
         <v>7</v>
       </c>
@@ -3895,7 +3625,7 @@
         <v>174</v>
       </c>
       <c r="F44" s="46" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>413</v>
@@ -3915,14 +3645,8 @@
       <c r="L44" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="M44" s="31"/>
-      <c r="N44" s="31"/>
-      <c r="O44" s="31"/>
-      <c r="P44" s="31"/>
-      <c r="Q44" s="31"/>
-      <c r="R44" s="31"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="45" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>8</v>
       </c>
@@ -3939,7 +3663,7 @@
         <v>174</v>
       </c>
       <c r="F45" s="46" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>414</v>
@@ -3959,14 +3683,8 @@
       <c r="L45" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="46" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>8</v>
       </c>
@@ -3983,7 +3701,7 @@
         <v>174</v>
       </c>
       <c r="F46" s="46" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>414</v>
@@ -4003,14 +3721,8 @@
       <c r="L46" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="47" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>8</v>
       </c>
@@ -4027,7 +3739,7 @@
         <v>174</v>
       </c>
       <c r="F47" s="46" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>414</v>
@@ -4047,14 +3759,8 @@
       <c r="L47" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="48" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>8</v>
       </c>
@@ -4071,7 +3777,7 @@
         <v>174</v>
       </c>
       <c r="F48" s="46" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>414</v>
@@ -4091,14 +3797,8 @@
       <c r="L48" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="49" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>8</v>
       </c>
@@ -4115,7 +3815,7 @@
         <v>174</v>
       </c>
       <c r="F49" s="46" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>414</v>
@@ -4135,14 +3835,8 @@
       <c r="L49" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="50" s="31" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="31">
         <v>8</v>
       </c>
@@ -4159,7 +3853,7 @@
         <v>174</v>
       </c>
       <c r="F50" s="46" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>414</v>
@@ -4179,14 +3873,8 @@
       <c r="L50" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="M50" s="31"/>
-      <c r="N50" s="31"/>
-      <c r="O50" s="31"/>
-      <c r="P50" s="31"/>
-      <c r="Q50" s="31"/>
-      <c r="R50" s="31"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="51" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="44">
         <v>9</v>
       </c>
@@ -4203,19 +3891,19 @@
         <v>174</v>
       </c>
       <c r="F51" s="46" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>226</v>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
+      <c r="J51" s="3">
+        <v>0</v>
       </c>
       <c r="K51" s="30" t="s">
         <v>2</v>
@@ -4223,14 +3911,8 @@
       <c r="L51" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="52" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="44">
         <v>9</v>
       </c>
@@ -4247,19 +3929,19 @@
         <v>174</v>
       </c>
       <c r="F52" s="46" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="H52" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>226</v>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0</v>
       </c>
       <c r="K52" s="30" t="s">
         <v>2</v>
@@ -4267,14 +3949,8 @@
       <c r="L52" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="53" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="44">
         <v>9</v>
       </c>
@@ -4291,19 +3967,19 @@
         <v>174</v>
       </c>
       <c r="F53" s="46" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="H53" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>226</v>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
+        <v>0</v>
+      </c>
+      <c r="J53" s="3">
+        <v>0</v>
       </c>
       <c r="K53" s="30" t="s">
         <v>2</v>
@@ -4311,14 +3987,8 @@
       <c r="L53" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
-      <c r="R53" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="54" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="44">
         <v>9</v>
       </c>
@@ -4335,19 +4005,19 @@
         <v>174</v>
       </c>
       <c r="F54" s="46" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="H54" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>226</v>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0</v>
+      </c>
+      <c r="J54" s="3">
+        <v>0</v>
       </c>
       <c r="K54" s="30" t="s">
         <v>2</v>
@@ -4355,14 +4025,8 @@
       <c r="L54" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-      <c r="Q54" s="3"/>
-      <c r="R54" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="55" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="44">
         <v>9</v>
       </c>
@@ -4379,19 +4043,19 @@
         <v>174</v>
       </c>
       <c r="F55" s="46" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="H55" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>226</v>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3">
+        <v>0</v>
       </c>
       <c r="K55" s="30" t="s">
         <v>2</v>
@@ -4399,14 +4063,8 @@
       <c r="L55" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="56" s="31" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="31">
         <v>9</v>
       </c>
@@ -4423,19 +4081,19 @@
         <v>174</v>
       </c>
       <c r="F56" s="46" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="H56" s="40" t="s">
-        <v>423</v>
-      </c>
-      <c r="I56" s="40" t="s">
-        <v>226</v>
-      </c>
-      <c r="J56" s="40" t="s">
-        <v>226</v>
+      <c r="H56" s="40">
+        <v>0</v>
+      </c>
+      <c r="I56" s="40">
+        <v>0</v>
+      </c>
+      <c r="J56" s="40">
+        <v>0</v>
       </c>
       <c r="K56" s="31" t="s">
         <v>2</v>
@@ -4443,14 +4101,8 @@
       <c r="L56" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="M56" s="31"/>
-      <c r="N56" s="31"/>
-      <c r="O56" s="31"/>
-      <c r="P56" s="31"/>
-      <c r="Q56" s="31"/>
-      <c r="R56" s="31"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="57" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="44">
         <v>10</v>
       </c>
@@ -4487,14 +4139,8 @@
       <c r="L57" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
-      <c r="R57" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="58" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="44">
         <v>10</v>
       </c>
@@ -4531,14 +4177,8 @@
       <c r="L58" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
-      <c r="R58" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="59" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="44">
         <v>10</v>
       </c>
@@ -4575,14 +4215,8 @@
       <c r="L59" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
-      <c r="O59" s="3"/>
-      <c r="P59" s="3"/>
-      <c r="Q59" s="3"/>
-      <c r="R59" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="60" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="44">
         <v>10</v>
       </c>
@@ -4619,14 +4253,8 @@
       <c r="L60" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M60" s="3"/>
-      <c r="N60" s="3"/>
-      <c r="O60" s="3"/>
-      <c r="P60" s="3"/>
-      <c r="Q60" s="3"/>
-      <c r="R60" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="61" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="44">
         <v>10</v>
       </c>
@@ -4663,14 +4291,8 @@
       <c r="L61" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M61" s="3"/>
-      <c r="N61" s="3"/>
-      <c r="O61" s="3"/>
-      <c r="P61" s="3"/>
-      <c r="Q61" s="3"/>
-      <c r="R61" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="62" s="31" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="31">
         <v>10</v>
       </c>
@@ -4707,14 +4329,8 @@
       <c r="L62" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="M62" s="31"/>
-      <c r="N62" s="31"/>
-      <c r="O62" s="31"/>
-      <c r="P62" s="31"/>
-      <c r="Q62" s="31"/>
-      <c r="R62" s="31"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="63" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="44">
         <v>11</v>
       </c>
@@ -4751,14 +4367,8 @@
       <c r="L63" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M63" s="3"/>
-      <c r="N63" s="3"/>
-      <c r="O63" s="3"/>
-      <c r="P63" s="3"/>
-      <c r="Q63" s="3"/>
-      <c r="R63" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="64" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="44">
         <v>11</v>
       </c>
@@ -4795,14 +4405,8 @@
       <c r="L64" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M64" s="3"/>
-      <c r="N64" s="3"/>
-      <c r="O64" s="3"/>
-      <c r="P64" s="3"/>
-      <c r="Q64" s="3"/>
-      <c r="R64" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="65" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="44">
         <v>11</v>
       </c>
@@ -4839,14 +4443,8 @@
       <c r="L65" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
-      <c r="O65" s="3"/>
-      <c r="P65" s="3"/>
-      <c r="Q65" s="3"/>
-      <c r="R65" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="66" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="44">
         <v>11</v>
       </c>
@@ -4883,14 +4481,8 @@
       <c r="L66" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
-      <c r="O66" s="3"/>
-      <c r="P66" s="3"/>
-      <c r="Q66" s="3"/>
-      <c r="R66" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="67" s="3" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="44">
         <v>11</v>
       </c>
@@ -4927,14 +4519,8 @@
       <c r="L67" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M67" s="3"/>
-      <c r="N67" s="3"/>
-      <c r="O67" s="3"/>
-      <c r="P67" s="3"/>
-      <c r="Q67" s="3"/>
-      <c r="R67" s="3"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="68" s="31" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="31">
         <v>11</v>
       </c>
@@ -4971,14 +4557,8 @@
       <c r="L68" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="M68" s="31"/>
-      <c r="N68" s="31"/>
-      <c r="O68" s="31"/>
-      <c r="P68" s="31"/>
-      <c r="Q68" s="31"/>
-      <c r="R68" s="31"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="69" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>12</v>
       </c>
@@ -5015,14 +4595,8 @@
       <c r="L69" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M69" s="4"/>
-      <c r="N69" s="3"/>
-      <c r="O69" s="0"/>
-      <c r="P69" s="3"/>
-      <c r="Q69" s="3"/>
-      <c r="R69" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="70" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>12</v>
       </c>
@@ -5059,14 +4633,8 @@
       <c r="L70" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M70" s="4"/>
-      <c r="N70" s="3"/>
-      <c r="O70" s="0"/>
-      <c r="P70" s="3"/>
-      <c r="Q70" s="3"/>
-      <c r="R70" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="71" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>12</v>
       </c>
@@ -5103,14 +4671,8 @@
       <c r="L71" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M71" s="4"/>
-      <c r="N71" s="3"/>
-      <c r="O71" s="0"/>
-      <c r="P71" s="3"/>
-      <c r="Q71" s="3"/>
-      <c r="R71" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="72" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>12</v>
       </c>
@@ -5147,14 +4709,8 @@
       <c r="L72" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M72" s="4"/>
-      <c r="N72" s="3"/>
-      <c r="O72" s="0"/>
-      <c r="P72" s="3"/>
-      <c r="Q72" s="3"/>
-      <c r="R72" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="73" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>12</v>
       </c>
@@ -5191,14 +4747,8 @@
       <c r="L73" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M73" s="4"/>
-      <c r="N73" s="3"/>
-      <c r="O73" s="0"/>
-      <c r="P73" s="3"/>
-      <c r="Q73" s="3"/>
-      <c r="R73" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="74" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>12</v>
       </c>
@@ -5235,14 +4785,8 @@
       <c r="L74" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="M74" s="40"/>
-      <c r="N74" s="40"/>
-      <c r="O74" s="40"/>
-      <c r="P74" s="40"/>
-      <c r="Q74" s="40"/>
-      <c r="R74" s="40"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>13</v>
       </c>
@@ -5279,14 +4823,8 @@
       <c r="L75" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M75" s="4"/>
-      <c r="N75" s="3"/>
-      <c r="O75" s="0"/>
-      <c r="P75" s="3"/>
-      <c r="Q75" s="3"/>
-      <c r="R75" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="76" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>13</v>
       </c>
@@ -5323,14 +4861,8 @@
       <c r="L76" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M76" s="4"/>
-      <c r="N76" s="3"/>
-      <c r="O76" s="0"/>
-      <c r="P76" s="3"/>
-      <c r="Q76" s="3"/>
-      <c r="R76" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="77" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>13</v>
       </c>
@@ -5367,14 +4899,8 @@
       <c r="L77" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M77" s="4"/>
-      <c r="N77" s="3"/>
-      <c r="O77" s="0"/>
-      <c r="P77" s="3"/>
-      <c r="Q77" s="3"/>
-      <c r="R77" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="78" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>13</v>
       </c>
@@ -5411,14 +4937,8 @@
       <c r="L78" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M78" s="4"/>
-      <c r="N78" s="3"/>
-      <c r="O78" s="0"/>
-      <c r="P78" s="3"/>
-      <c r="Q78" s="3"/>
-      <c r="R78" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>13</v>
       </c>
@@ -5455,14 +4975,8 @@
       <c r="L79" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M79" s="4"/>
-      <c r="N79" s="3"/>
-      <c r="O79" s="0"/>
-      <c r="P79" s="3"/>
-      <c r="Q79" s="3"/>
-      <c r="R79" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="80" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>13</v>
       </c>
@@ -5499,14 +5013,8 @@
       <c r="L80" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="M80" s="40"/>
-      <c r="N80" s="40"/>
-      <c r="O80" s="40"/>
-      <c r="P80" s="40"/>
-      <c r="Q80" s="40"/>
-      <c r="R80" s="40"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="81" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>14</v>
       </c>
@@ -5543,14 +5051,8 @@
       <c r="L81" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M81" s="4"/>
-      <c r="N81" s="3"/>
-      <c r="O81" s="0"/>
-      <c r="P81" s="3"/>
-      <c r="Q81" s="3"/>
-      <c r="R81" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="82" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>14</v>
       </c>
@@ -5587,14 +5089,8 @@
       <c r="L82" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M82" s="4"/>
-      <c r="N82" s="3"/>
-      <c r="O82" s="0"/>
-      <c r="P82" s="3"/>
-      <c r="Q82" s="3"/>
-      <c r="R82" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="83" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>14</v>
       </c>
@@ -5631,14 +5127,8 @@
       <c r="L83" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M83" s="4"/>
-      <c r="N83" s="3"/>
-      <c r="O83" s="0"/>
-      <c r="P83" s="3"/>
-      <c r="Q83" s="3"/>
-      <c r="R83" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="84" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>14</v>
       </c>
@@ -5675,14 +5165,8 @@
       <c r="L84" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M84" s="4"/>
-      <c r="N84" s="3"/>
-      <c r="O84" s="0"/>
-      <c r="P84" s="3"/>
-      <c r="Q84" s="3"/>
-      <c r="R84" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>14</v>
       </c>
@@ -5719,14 +5203,8 @@
       <c r="L85" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M85" s="4"/>
-      <c r="N85" s="3"/>
-      <c r="O85" s="0"/>
-      <c r="P85" s="3"/>
-      <c r="Q85" s="3"/>
-      <c r="R85" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="86" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>14</v>
       </c>
@@ -5763,14 +5241,8 @@
       <c r="L86" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M86" s="40"/>
-      <c r="N86" s="40"/>
-      <c r="O86" s="40"/>
-      <c r="P86" s="40"/>
-      <c r="Q86" s="40"/>
-      <c r="R86" s="40"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="87" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>15</v>
       </c>
@@ -5807,14 +5279,8 @@
       <c r="L87" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M87" s="4"/>
-      <c r="N87" s="3"/>
-      <c r="O87" s="0"/>
-      <c r="P87" s="3"/>
-      <c r="Q87" s="3"/>
-      <c r="R87" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="88" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>15</v>
       </c>
@@ -5851,14 +5317,8 @@
       <c r="L88" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="M88" s="4"/>
-      <c r="N88" s="3"/>
-      <c r="O88" s="0"/>
-      <c r="P88" s="3"/>
-      <c r="Q88" s="3"/>
-      <c r="R88" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="89" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>15</v>
       </c>
@@ -5895,14 +5355,8 @@
       <c r="L89" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M89" s="4"/>
-      <c r="N89" s="3"/>
-      <c r="O89" s="0"/>
-      <c r="P89" s="3"/>
-      <c r="Q89" s="3"/>
-      <c r="R89" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="90" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>15</v>
       </c>
@@ -5939,14 +5393,8 @@
       <c r="L90" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M90" s="4"/>
-      <c r="N90" s="3"/>
-      <c r="O90" s="0"/>
-      <c r="P90" s="3"/>
-      <c r="Q90" s="3"/>
-      <c r="R90" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>15</v>
       </c>
@@ -5983,14 +5431,8 @@
       <c r="L91" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M91" s="4"/>
-      <c r="N91" s="3"/>
-      <c r="O91" s="0"/>
-      <c r="P91" s="3"/>
-      <c r="Q91" s="3"/>
-      <c r="R91" s="0"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="92" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>15</v>
       </c>
@@ -6027,14 +5469,8 @@
       <c r="L92" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="M92" s="40"/>
-      <c r="N92" s="40"/>
-      <c r="O92" s="40"/>
-      <c r="P92" s="40"/>
-      <c r="Q92" s="40"/>
-      <c r="R92" s="40"/>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="93" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B93" s="30"/>
       <c r="C93" s="13"/>
       <c r="D93" s="30"/>
@@ -6043,7 +5479,7 @@
       <c r="K93" s="30"/>
       <c r="L93" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="94" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B94" s="30"/>
       <c r="C94" s="30"/>
       <c r="D94" s="30"/>
@@ -6052,7 +5488,7 @@
       <c r="K94" s="30"/>
       <c r="L94" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="95" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B95" s="30"/>
       <c r="C95" s="3"/>
       <c r="D95" s="30"/>
@@ -6061,7 +5497,7 @@
       <c r="K95" s="30"/>
       <c r="L95" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="96" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B96" s="30"/>
       <c r="C96" s="30"/>
       <c r="D96" s="30"/>
@@ -6070,7 +5506,7 @@
       <c r="K96" s="30"/>
       <c r="L96" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="97" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B97" s="30"/>
       <c r="C97" s="30"/>
       <c r="D97" s="30"/>
@@ -6078,7 +5514,7 @@
       <c r="K97" s="30"/>
       <c r="L97" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="98" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3"/>
       <c r="B98" s="30"/>
       <c r="D98" s="30"/>
@@ -6087,7 +5523,7 @@
       <c r="K98" s="31"/>
       <c r="L98" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="99" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B99" s="30"/>
       <c r="C99" s="13"/>
       <c r="D99" s="30"/>
@@ -6096,7 +5532,7 @@
       <c r="K99" s="30"/>
       <c r="L99" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="100" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B100" s="30"/>
       <c r="C100" s="30"/>
       <c r="D100" s="30"/>
@@ -6105,7 +5541,7 @@
       <c r="K100" s="30"/>
       <c r="L100" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="101" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B101" s="30"/>
       <c r="C101" s="3"/>
       <c r="D101" s="30"/>
@@ -6114,7 +5550,7 @@
       <c r="K101" s="30"/>
       <c r="L101" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="102" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B102" s="30"/>
       <c r="C102" s="30"/>
       <c r="D102" s="30"/>
@@ -6123,7 +5559,7 @@
       <c r="K102" s="30"/>
       <c r="L102" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="103" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B103" s="30"/>
       <c r="C103" s="30"/>
       <c r="D103" s="30"/>
@@ -6132,7 +5568,7 @@
       <c r="K103" s="30"/>
       <c r="L103" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="104" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3"/>
       <c r="B104" s="30"/>
       <c r="D104" s="30"/>
@@ -6141,7 +5577,7 @@
       <c r="K104" s="31"/>
       <c r="L104" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="105" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B105" s="30"/>
       <c r="C105" s="13"/>
       <c r="D105" s="30"/>
@@ -6150,7 +5586,7 @@
       <c r="K105" s="30"/>
       <c r="L105" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="106" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B106" s="30"/>
       <c r="C106" s="30"/>
       <c r="D106" s="30"/>
@@ -6159,7 +5595,7 @@
       <c r="K106" s="30"/>
       <c r="L106" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="107" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B107" s="30"/>
       <c r="C107" s="3"/>
       <c r="D107" s="30"/>
@@ -6168,7 +5604,7 @@
       <c r="K107" s="30"/>
       <c r="L107" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="108" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B108" s="30"/>
       <c r="C108" s="30"/>
       <c r="D108" s="30"/>
@@ -6176,7 +5612,7 @@
       <c r="K108" s="30"/>
       <c r="L108" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="109" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B109" s="30"/>
       <c r="C109" s="30"/>
       <c r="D109" s="30"/>
@@ -6184,7 +5620,7 @@
       <c r="K109" s="30"/>
       <c r="L109" s="33"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="110" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3"/>
       <c r="B110" s="30"/>
       <c r="D110" s="30"/>
@@ -6193,7 +5629,7 @@
       <c r="K110" s="31"/>
       <c r="L110" s="35"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="111" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B111" s="30"/>
       <c r="C111" s="13"/>
       <c r="D111" s="30"/>
@@ -6202,7 +5638,7 @@
       <c r="K111" s="30"/>
       <c r="L111" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="112" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B112" s="30"/>
       <c r="C112" s="30"/>
       <c r="D112" s="30"/>
@@ -6211,7 +5647,7 @@
       <c r="K112" s="30"/>
       <c r="L112" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="113" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B113" s="30"/>
       <c r="C113" s="3"/>
       <c r="D113" s="30"/>
@@ -6220,7 +5656,7 @@
       <c r="K113" s="30"/>
       <c r="L113" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="114" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B114" s="30"/>
       <c r="C114" s="30"/>
       <c r="D114" s="30"/>
@@ -6229,7 +5665,7 @@
       <c r="K114" s="30"/>
       <c r="L114" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="115" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B115" s="30"/>
       <c r="C115" s="30"/>
       <c r="D115" s="30"/>
@@ -6238,7 +5674,7 @@
       <c r="K115" s="30"/>
       <c r="L115" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="116" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3"/>
       <c r="B116" s="30"/>
       <c r="D116" s="30"/>
@@ -6247,7 +5683,7 @@
       <c r="K116" s="31"/>
       <c r="L116" s="35"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="117" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B117" s="30"/>
       <c r="C117" s="13"/>
       <c r="D117" s="30"/>
@@ -6255,7 +5691,7 @@
       <c r="K117" s="30"/>
       <c r="L117" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="118" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B118" s="30"/>
       <c r="C118" s="30"/>
       <c r="D118" s="30"/>
@@ -6264,7 +5700,7 @@
       <c r="K118" s="30"/>
       <c r="L118" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="119" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B119" s="30"/>
       <c r="C119" s="3"/>
       <c r="D119" s="30"/>
@@ -6273,7 +5709,7 @@
       <c r="K119" s="30"/>
       <c r="L119" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="120" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B120" s="30"/>
       <c r="C120" s="30"/>
       <c r="D120" s="30"/>
@@ -6282,7 +5718,7 @@
       <c r="K120" s="30"/>
       <c r="L120" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="121" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B121" s="30"/>
       <c r="C121" s="30"/>
       <c r="D121" s="30"/>
@@ -6291,7 +5727,7 @@
       <c r="K121" s="30"/>
       <c r="L121" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="122" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3"/>
       <c r="B122" s="30"/>
       <c r="D122" s="30"/>
@@ -6300,7 +5736,7 @@
       <c r="K122" s="31"/>
       <c r="L122" s="35"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="123" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B123" s="30"/>
       <c r="C123" s="13"/>
       <c r="D123" s="30"/>
@@ -6308,7 +5744,7 @@
       <c r="K123" s="30"/>
       <c r="L123" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="124" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B124" s="30"/>
       <c r="C124" s="30"/>
       <c r="D124" s="30"/>
@@ -6317,7 +5753,7 @@
       <c r="K124" s="30"/>
       <c r="L124" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="125" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B125" s="30"/>
       <c r="C125" s="3"/>
       <c r="D125" s="30"/>
@@ -6326,7 +5762,7 @@
       <c r="K125" s="30"/>
       <c r="L125" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="126" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B126" s="30"/>
       <c r="C126" s="30"/>
       <c r="D126" s="30"/>
@@ -6335,7 +5771,7 @@
       <c r="K126" s="30"/>
       <c r="L126" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="127" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B127" s="30"/>
       <c r="C127" s="30"/>
       <c r="D127" s="30"/>
@@ -6344,7 +5780,7 @@
       <c r="K127" s="30"/>
       <c r="L127" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="128" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3"/>
       <c r="B128" s="30"/>
       <c r="D128" s="30"/>
@@ -6353,7 +5789,7 @@
       <c r="K128" s="31"/>
       <c r="L128" s="35"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="129" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B129" s="30"/>
       <c r="C129" s="13"/>
       <c r="D129" s="30"/>
@@ -6361,7 +5797,7 @@
       <c r="K129" s="30"/>
       <c r="L129" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="130" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B130" s="30"/>
       <c r="C130" s="30"/>
       <c r="D130" s="30"/>
@@ -6370,7 +5806,7 @@
       <c r="K130" s="30"/>
       <c r="L130" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="131" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B131" s="30"/>
       <c r="C131" s="3"/>
       <c r="D131" s="30"/>
@@ -6379,7 +5815,7 @@
       <c r="K131" s="30"/>
       <c r="L131" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="132" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B132" s="30"/>
       <c r="C132" s="30"/>
       <c r="D132" s="30"/>
@@ -6388,7 +5824,7 @@
       <c r="K132" s="30"/>
       <c r="L132" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="133" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B133" s="30"/>
       <c r="C133" s="30"/>
       <c r="D133" s="30"/>
@@ -6397,7 +5833,7 @@
       <c r="K133" s="30"/>
       <c r="L133" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="134" s="40" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3"/>
       <c r="B134" s="30"/>
       <c r="D134" s="30"/>
@@ -6406,7 +5842,7 @@
       <c r="K134" s="31"/>
       <c r="L134" s="35"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="135" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B135" s="30"/>
       <c r="C135" s="13"/>
       <c r="D135" s="30"/>
@@ -6415,7 +5851,7 @@
       <c r="K135" s="30"/>
       <c r="L135" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="136" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B136" s="30"/>
       <c r="C136" s="30"/>
       <c r="D136" s="30"/>
@@ -6424,7 +5860,7 @@
       <c r="K136" s="30"/>
       <c r="L136" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="137" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B137" s="30"/>
       <c r="C137" s="3"/>
       <c r="D137" s="30"/>
@@ -6433,7 +5869,7 @@
       <c r="K137" s="30"/>
       <c r="L137" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="138" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B138" s="30"/>
       <c r="C138" s="30"/>
       <c r="D138" s="30"/>
@@ -6442,7 +5878,7 @@
       <c r="K138" s="30"/>
       <c r="L138" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="139" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B139" s="30"/>
       <c r="C139" s="30"/>
       <c r="D139" s="30"/>
@@ -6451,7 +5887,7 @@
       <c r="K139" s="30"/>
       <c r="L139" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="140" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B140" s="30"/>
       <c r="C140" s="40"/>
       <c r="D140" s="30"/>
@@ -6463,7 +5899,7 @@
       <c r="K140" s="31"/>
       <c r="L140" s="35"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="141" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B141" s="30"/>
       <c r="C141" s="13"/>
       <c r="D141" s="30"/>
@@ -6471,7 +5907,7 @@
       <c r="K141" s="30"/>
       <c r="L141" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="142" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B142" s="30"/>
       <c r="C142" s="30"/>
       <c r="D142" s="30"/>
@@ -6479,7 +5915,7 @@
       <c r="K142" s="30"/>
       <c r="L142" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="143" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B143" s="30"/>
       <c r="C143" s="3"/>
       <c r="D143" s="30"/>
@@ -6488,7 +5924,7 @@
       <c r="K143" s="30"/>
       <c r="L143" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="144" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B144" s="30"/>
       <c r="C144" s="30"/>
       <c r="D144" s="30"/>
@@ -6497,7 +5933,7 @@
       <c r="K144" s="30"/>
       <c r="L144" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="145" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B145" s="30"/>
       <c r="C145" s="30"/>
       <c r="D145" s="30"/>
@@ -6506,7 +5942,7 @@
       <c r="K145" s="30"/>
       <c r="L145" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="146" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B146" s="30"/>
       <c r="C146" s="40"/>
       <c r="D146" s="30"/>
@@ -6518,7 +5954,7 @@
       <c r="K146" s="31"/>
       <c r="L146" s="35"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="147" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B147" s="30"/>
       <c r="C147" s="13"/>
       <c r="D147" s="30"/>
@@ -6526,7 +5962,7 @@
       <c r="K147" s="30"/>
       <c r="L147" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="148" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B148" s="30"/>
       <c r="C148" s="30"/>
       <c r="D148" s="30"/>
@@ -6534,7 +5970,7 @@
       <c r="K148" s="30"/>
       <c r="L148" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="149" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B149" s="30"/>
       <c r="C149" s="3"/>
       <c r="D149" s="30"/>
@@ -6543,7 +5979,7 @@
       <c r="K149" s="30"/>
       <c r="L149" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="150" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B150" s="30"/>
       <c r="C150" s="30"/>
       <c r="D150" s="30"/>
@@ -6552,7 +5988,7 @@
       <c r="K150" s="30"/>
       <c r="L150" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="151" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B151" s="30"/>
       <c r="C151" s="30"/>
       <c r="D151" s="30"/>
@@ -6561,7 +5997,7 @@
       <c r="K151" s="30"/>
       <c r="L151" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="152" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B152" s="30"/>
       <c r="C152" s="40"/>
       <c r="D152" s="30"/>
@@ -6573,7 +6009,7 @@
       <c r="K152" s="31"/>
       <c r="L152" s="35"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="153" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B153" s="30"/>
       <c r="C153" s="13"/>
       <c r="D153" s="30"/>
@@ -6581,7 +6017,7 @@
       <c r="K153" s="30"/>
       <c r="L153" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="154" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B154" s="30"/>
       <c r="C154" s="30"/>
       <c r="D154" s="30"/>
@@ -6590,7 +6026,7 @@
       <c r="K154" s="30"/>
       <c r="L154" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="155" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B155" s="30"/>
       <c r="C155" s="3"/>
       <c r="D155" s="30"/>
@@ -6599,7 +6035,7 @@
       <c r="K155" s="30"/>
       <c r="L155" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="156" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B156" s="30"/>
       <c r="C156" s="30"/>
       <c r="D156" s="30"/>
@@ -6608,7 +6044,7 @@
       <c r="K156" s="30"/>
       <c r="L156" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="157" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B157" s="30"/>
       <c r="C157" s="30"/>
       <c r="D157" s="30"/>
@@ -6617,7 +6053,7 @@
       <c r="K157" s="30"/>
       <c r="L157" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="158" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B158" s="30"/>
       <c r="C158" s="40"/>
       <c r="D158" s="30"/>
@@ -6629,7 +6065,7 @@
       <c r="K158" s="31"/>
       <c r="L158" s="35"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="159" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B159" s="30"/>
       <c r="C159" s="13"/>
       <c r="D159" s="30"/>
@@ -6637,7 +6073,7 @@
       <c r="K159" s="30"/>
       <c r="L159" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="160" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B160" s="30"/>
       <c r="C160" s="30"/>
       <c r="D160" s="30"/>
@@ -6646,7 +6082,7 @@
       <c r="K160" s="30"/>
       <c r="L160" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="161" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B161" s="30"/>
       <c r="C161" s="3"/>
       <c r="D161" s="30"/>
@@ -6655,7 +6091,7 @@
       <c r="K161" s="30"/>
       <c r="L161" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="162" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B162" s="30"/>
       <c r="C162" s="30"/>
       <c r="D162" s="30"/>
@@ -6664,7 +6100,7 @@
       <c r="K162" s="30"/>
       <c r="L162" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="163" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B163" s="30"/>
       <c r="C163" s="30"/>
       <c r="D163" s="30"/>
@@ -6673,7 +6109,7 @@
       <c r="K163" s="30"/>
       <c r="L163" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="164" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B164" s="30"/>
       <c r="C164" s="40"/>
       <c r="D164" s="30"/>
@@ -6685,32 +6121,32 @@
       <c r="K164" s="31"/>
       <c r="L164" s="35"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="165" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C165" s="13"/>
       <c r="K165" s="30"/>
       <c r="L165" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="166" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C166" s="30"/>
       <c r="K166" s="30"/>
       <c r="L166" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="167" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C167" s="3"/>
       <c r="K167" s="30"/>
       <c r="L167" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="168" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C168" s="30"/>
       <c r="K168" s="30"/>
       <c r="L168" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="169" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C169" s="30"/>
       <c r="K169" s="30"/>
       <c r="L169" s="32"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="170" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C170" s="40"/>
       <c r="H170" s="40"/>
       <c r="I170" s="40"/>
@@ -6726,27 +6162,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF2ED278-273F-4F08-AE25-85403C7565F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF2ED278-273F-4F08-AE25-85403C7565F1}">
   <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.625" style="19" customWidth="true"/>
-    <col min="2" max="2" width="63.375" style="19" customWidth="true"/>
-    <col min="3" max="3" width="30.25" style="19" customWidth="true"/>
-    <col min="4" max="4" width="72.75" style="19" customWidth="true"/>
-    <col min="5" max="5" width="10.625" style="19" customWidth="true"/>
-    <col min="6" max="6" width="14.25" style="19" customWidth="true"/>
+    <col min="1" max="1" width="15.625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="63.375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="30.25" style="19" customWidth="1"/>
+    <col min="4" max="4" width="72.75" style="19" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="14.25" style="19" customWidth="1"/>
     <col min="7" max="8" width="8.875" style="19"/>
-    <col min="9" max="9" width="9" style="22" customWidth="true"/>
+    <col min="9" max="9" width="9" style="22" customWidth="1"/>
     <col min="10" max="16384" width="8.875" style="19"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="9" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24">
         <v>43</v>
       </c>
@@ -6788,7 +6224,7 @@
       <c r="P1" s="13"/>
       <c r="Q1" s="13"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="25">
         <v>43</v>
       </c>
@@ -6830,7 +6266,7 @@
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="25">
         <v>43</v>
       </c>
@@ -6872,7 +6308,7 @@
       <c r="P3" s="22"/>
       <c r="Q3" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>43</v>
       </c>
@@ -6910,7 +6346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>43</v>
       </c>
@@ -6948,7 +6384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>43</v>
       </c>
@@ -6986,7 +6422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" s="14" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
         <v>43</v>
       </c>
@@ -7024,7 +6460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" s="9" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24">
         <v>44</v>
       </c>
@@ -7066,7 +6502,7 @@
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="25">
         <v>44</v>
       </c>
@@ -7108,7 +6544,7 @@
       <c r="P9" s="22"/>
       <c r="Q9" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="25">
         <v>44</v>
       </c>
@@ -7150,7 +6586,7 @@
       <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="23">
         <v>44</v>
       </c>
@@ -7188,7 +6624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="23">
         <v>44</v>
       </c>
@@ -7226,7 +6662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="23">
         <v>44</v>
       </c>
@@ -7264,7 +6700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" s="14" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="26">
         <v>44</v>
       </c>
@@ -7302,7 +6738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" s="9" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24">
         <v>45</v>
       </c>
@@ -7344,7 +6780,7 @@
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="25">
         <v>45</v>
       </c>
@@ -7386,7 +6822,7 @@
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="25">
         <v>45</v>
       </c>
@@ -7428,7 +6864,7 @@
       <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="23">
         <v>45</v>
       </c>
@@ -7466,7 +6902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="23">
         <v>45</v>
       </c>
@@ -7504,7 +6940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="23">
         <v>45</v>
       </c>
@@ -7542,7 +6978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" s="14" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="26">
         <v>45</v>
       </c>
@@ -7580,7 +7016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" s="9" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="24">
         <v>46</v>
       </c>
@@ -7622,7 +7058,7 @@
       <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="25">
         <v>46</v>
       </c>
@@ -7664,7 +7100,7 @@
       <c r="P23" s="22"/>
       <c r="Q23" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="25">
         <v>46</v>
       </c>
@@ -7706,7 +7142,7 @@
       <c r="P24" s="22"/>
       <c r="Q24" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="23">
         <v>46</v>
       </c>
@@ -7744,7 +7180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="23">
         <v>46</v>
       </c>
@@ -7782,7 +7218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="23">
         <v>46</v>
       </c>
@@ -7820,7 +7256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" s="14" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="26">
         <v>46</v>
       </c>
@@ -7858,7 +7294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="29" s="9" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="24">
         <v>47</v>
       </c>
@@ -7900,7 +7336,7 @@
       <c r="P29" s="13"/>
       <c r="Q29" s="13"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="25">
         <v>47</v>
       </c>
@@ -7942,7 +7378,7 @@
       <c r="P30" s="22"/>
       <c r="Q30" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="31" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="25">
         <v>47</v>
       </c>
@@ -7984,7 +7420,7 @@
       <c r="P31" s="22"/>
       <c r="Q31" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="23">
         <v>47</v>
       </c>
@@ -8022,7 +7458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="33" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="23">
         <v>47</v>
       </c>
@@ -8060,7 +7496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="23">
         <v>47</v>
       </c>
@@ -8098,7 +7534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="35" s="14" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="26">
         <v>47</v>
       </c>
@@ -8136,7 +7572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="36" s="9" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="24">
         <v>48</v>
       </c>
@@ -8178,7 +7614,7 @@
       <c r="P36" s="13"/>
       <c r="Q36" s="13"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="37" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="25">
         <v>48</v>
       </c>
@@ -8220,7 +7656,7 @@
       <c r="P37" s="22"/>
       <c r="Q37" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="38" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="25">
         <v>48</v>
       </c>
@@ -8262,7 +7698,7 @@
       <c r="P38" s="22"/>
       <c r="Q38" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="39" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="23">
         <v>48</v>
       </c>
@@ -8300,7 +7736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="23">
         <v>48</v>
       </c>
@@ -8338,7 +7774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="41" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="23">
         <v>48</v>
       </c>
@@ -8376,7 +7812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="42" s="14" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="26">
         <v>48</v>
       </c>
@@ -8414,7 +7850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="43" s="9" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="24">
         <v>49</v>
       </c>
@@ -8456,7 +7892,7 @@
       <c r="P43" s="13"/>
       <c r="Q43" s="13"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="44" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="25">
         <v>49</v>
       </c>
@@ -8498,7 +7934,7 @@
       <c r="P44" s="22"/>
       <c r="Q44" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="45" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="25">
         <v>49</v>
       </c>
@@ -8540,7 +7976,7 @@
       <c r="P45" s="22"/>
       <c r="Q45" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="46" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="23">
         <v>49</v>
       </c>
@@ -8578,7 +8014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="47" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="23">
         <v>49</v>
       </c>
@@ -8616,7 +8052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="48" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="23">
         <v>49</v>
       </c>
@@ -8654,7 +8090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="49" s="14" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="26">
         <v>49</v>
       </c>
@@ -8692,7 +8128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="50" s="9" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="24">
         <v>50</v>
       </c>
@@ -8734,7 +8170,7 @@
       <c r="P50" s="13"/>
       <c r="Q50" s="13"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="51" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="25">
         <v>50</v>
       </c>
@@ -8776,7 +8212,7 @@
       <c r="P51" s="22"/>
       <c r="Q51" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="52" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="25">
         <v>50</v>
       </c>
@@ -8818,7 +8254,7 @@
       <c r="P52" s="22"/>
       <c r="Q52" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="53" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="23">
         <v>50</v>
       </c>
@@ -8856,7 +8292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="54" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="23">
         <v>50</v>
       </c>
@@ -8894,7 +8330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="55" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="23">
         <v>50</v>
       </c>
@@ -8932,7 +8368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="56" s="14" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="26">
         <v>50</v>
       </c>
@@ -8970,7 +8406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="57" s="9" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="24">
         <v>51</v>
       </c>
@@ -9012,7 +8448,7 @@
       <c r="P57" s="13"/>
       <c r="Q57" s="13"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="58" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="25">
         <v>51</v>
       </c>
@@ -9054,7 +8490,7 @@
       <c r="P58" s="22"/>
       <c r="Q58" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="59" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="25">
         <v>51</v>
       </c>
@@ -9096,7 +8532,7 @@
       <c r="P59" s="22"/>
       <c r="Q59" s="22"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="60" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="23">
         <v>51</v>
       </c>
@@ -9134,7 +8570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="61" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="23">
         <v>51</v>
       </c>
@@ -9172,7 +8608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="62" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="23">
         <v>51</v>
       </c>
@@ -9210,7 +8646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="63" s="14" customFormat="true" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="26">
         <v>51</v>
       </c>
@@ -9256,25 +8692,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BBBC03-E097-4F2C-B05D-E35D590A3209}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BBBC03-E097-4F2C-B05D-E35D590A3209}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" style="28"/>
-    <col min="2" max="2" width="69.25" style="28" customWidth="true"/>
-    <col min="3" max="3" width="33.375" style="28" customWidth="true"/>
-    <col min="4" max="4" width="69.25" style="28" customWidth="true"/>
+    <col min="2" max="2" width="69.25" style="28" customWidth="1"/>
+    <col min="3" max="3" width="33.375" style="28" customWidth="1"/>
+    <col min="4" max="4" width="69.25" style="28" customWidth="1"/>
     <col min="5" max="5" width="8.875" style="28"/>
-    <col min="6" max="6" width="17.25" style="28" customWidth="true"/>
+    <col min="6" max="6" width="17.25" style="28" customWidth="1"/>
     <col min="7" max="16384" width="8.875" style="28"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="28">
         <v>126</v>
       </c>
@@ -9312,7 +8748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="28">
         <v>126</v>
       </c>
@@ -9350,7 +8786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="28">
         <v>126</v>
       </c>
@@ -9388,7 +8824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="28">
         <v>126</v>
       </c>
@@ -9426,7 +8862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="28">
         <v>126</v>
       </c>
@@ -9464,7 +8900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="28">
         <v>126</v>
       </c>
@@ -9502,7 +8938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="28">
         <v>127</v>
       </c>
@@ -9540,7 +8976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="28">
         <v>127</v>
       </c>
@@ -9578,7 +9014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="28">
         <v>127</v>
       </c>
@@ -9616,7 +9052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="28">
         <v>127</v>
       </c>
@@ -9654,7 +9090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="28">
         <v>127</v>
       </c>
@@ -9692,7 +9128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="28">
         <v>127</v>
       </c>
@@ -9730,7 +9166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="28">
         <v>128</v>
       </c>
@@ -9768,7 +9204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="28">
         <v>128</v>
       </c>
@@ -9806,7 +9242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="28">
         <v>128</v>
       </c>
@@ -9844,7 +9280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="28">
         <v>128</v>
       </c>
@@ -9882,7 +9318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="28">
         <v>128</v>
       </c>
@@ -9920,7 +9356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="28">
         <v>128</v>
       </c>
@@ -9958,31 +9394,31 @@
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E19" s="29"/>
       <c r="N19" s="29"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="29"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E20" s="29"/>
       <c r="N20" s="29"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="29"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E21" s="29"/>
       <c r="N21" s="29"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="29"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E22" s="29"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" ht="11.25" customHeight="true" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E23" s="29"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" ht="11.25" customHeight="true" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E24" s="29"/>
     </row>
   </sheetData>

</xml_diff>